<commit_message>
updated sqlite tables, and sqlite queries
</commit_message>
<xml_diff>
--- a/prep_and_checklists/Samantha Remy/PREPLIST_Samantha Remy_06-20-2025_0.xlsx
+++ b/prep_and_checklists/Samantha Remy/PREPLIST_Samantha Remy_06-20-2025_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcuvin/purveyor_project/prep_and_checklists/Samantha Remy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B899F56E-B398-934B-9417-3EEFAEB526BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACF3757-DA6E-5A4F-8FA9-DD8E6E1860C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32980" yWindow="80" windowWidth="30240" windowHeight="17980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35760" yWindow="-220" windowWidth="30240" windowHeight="17980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prep_sheet" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="158">
   <si>
     <t>Samantha Remy 28 Guests 6:00 PM - 10:00 PM Friday, June 27, 2025</t>
   </si>
@@ -505,13 +505,16 @@
   </si>
   <si>
     <t>28 each</t>
+  </si>
+  <si>
+    <t>Canape</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -559,8 +562,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -571,6 +581,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
         <bgColor rgb="FFD3D3D3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -601,7 +617,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -613,6 +629,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -915,10 +935,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -948,7 +971,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
+      <c r="A5" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5" s="8"/>
       <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:5" ht="19" x14ac:dyDescent="0.2">
@@ -1018,6 +1044,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
       <c r="D11" s="3" t="s">
         <v>36</v>
       </c>
@@ -1128,6 +1156,8 @@
       <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
       <c r="D21" s="2" t="s">
         <v>131</v>
       </c>
@@ -1211,6 +1241,10 @@
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+    </row>
     <row r="29" spans="1:5" ht="19" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>20</v>
@@ -1278,6 +1312,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="19" x14ac:dyDescent="0.2">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
       <c r="D34" s="3" t="s">
         <v>47</v>
       </c>
@@ -1460,8 +1496,11 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup scale="45" orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -1928,5 +1967,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>